<commit_message>
refactor: make draw text more general
</commit_message>
<xml_diff>
--- a/stimuli_toy/multipleye_stimuli_experiment_toy.xlsx
+++ b/stimuli_toy/multipleye_stimuli_experiment_toy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-image-creation/stimuli_toy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653D444E-243D-2A4E-8F5E-60815E0E0CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7CA67F-50EE-D240-B9AF-CB1A705D2B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{EF339F11-F4DE-4D0A-862E-E00578AF5D2A}"/>
+    <workbookView xWindow="51200" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EF339F11-F4DE-4D0A-862E-E00578AF5D2A}"/>
   </bookViews>
   <sheets>
     <sheet name="PopSci_MultiplEYE_EN_example_st" sheetId="2" r:id="rId1"/>
@@ -146,13 +146,13 @@
     <t xml:space="preserve">Eye movements in reading are known to reflect cognitive processes involved in reading comprehension at all linguistic levels, from the sub-lexical to the discourse level. This means that reading comprehension and other properties of the text and/or the reader should be possible to infer from eye movements. Consequently, we develop the first neural sequence architecture for this type of tasks which models scan paths in reading and incorporates lexical, semantic and other linguistic features of the stimulus text. Our proposed model outperforms state-of-the-art models in various tasks. </t>
   </si>
   <si>
-    <t>toy_text_practice_1</t>
-  </si>
-  <si>
     <t>This was the happy side of the house, for the south and east looked rather melancholy even under the brightest morning. The grounds here were more confined, the flower-beds showed no very careful tendance, and large clumps of trees, chiefly of sombre yews, had risen high, not ten yards from the windows. The building, of greenish stone, was in the old English style, not ugly, but small-windowed and melancholy-looking: the sort of house that must have children, many flowers, open windows, and little vistas of bright things, to make it seem a joyous home.</t>
   </si>
   <si>
     <t>zuz</t>
+  </si>
+  <si>
+    <t>toy_text_3</t>
   </si>
 </sst>
 </file>
@@ -727,7 +727,7 @@
   <dimension ref="A1:BU17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -961,18 +961,18 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:73" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:73" x14ac:dyDescent="0.2">

</xml_diff>